<commit_message>
Updaate to capture models and fix reviews.
</commit_message>
<xml_diff>
--- a/GenericScenarioEvaluation/Reviewed Scenarios/BB/Chemical Additives Used in Automotive Lubricants Draft.xlsx
+++ b/GenericScenarioEvaluation/Reviewed Scenarios/BB/Chemical Additives Used in Automotive Lubricants Draft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/barrett_williamm_epa_gov/Documents/Profile/Desktop/GS Review/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WBARRETT\Environmental Protection Agency (EPA)\CSS RA-2 Project Team - General\Bill Paper - Generic Scenario Review\Reviewed Scenarios\BB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="8_{D21B3DA9-9B20-429C-8408-69FD36AE1659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{8EBF0ECE-1C48-48A5-AD4B-122EA851E493}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53449CE7-5C54-45F0-8381-3EDA81C7B7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AEE7231D-D110-46BA-BB08-35ECB9C6F51B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AEE7231D-D110-46BA-BB08-35ECB9C6F51B}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="358">
   <si>
     <t>Included? (Y or N)</t>
   </si>
@@ -1577,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A8DA8E-F055-4EAE-98B3-B13E29507A62}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1789,11 +1789,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE2C11F-6A25-4CA6-B493-2A0028270B50}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1856,9 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="H2" s="7"/>
       <c r="I2" t="s">
         <v>62</v>
@@ -3507,8 +3509,61 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F11D2A2FBBEED40A750386529AFE883" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a7fcd2fa88e0328b3b0dd9ef335fe48c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="241d41d8-5778-4e30-b44e-dee891c66b79" xmlns:ns6="af43f131-d884-42a1-ba66-3c1404ec48fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a2a87f8101accce6a0d0ea40fd00900" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2021-03-04T14:13:47+00:00</Document_x0020_Creation_x0020_Date>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F11D2A2FBBEED40A750386529AFE883" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2aa3aab08a376cfae5285fd06ce1ffe6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="241d41d8-5778-4e30-b44e-dee891c66b79" xmlns:ns6="af43f131-d884-42a1-ba66-3c1404ec48fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3082f80a83a1e1c83f67dad1a9ae4a33" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint.v3"/>
@@ -3548,6 +3603,8 @@
                 <xsd:element ref="ns5:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns5:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns5:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3809,6 +3866,16 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="38" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="39" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="af43f131-d884-42a1-ba66-3c1404ec48fc" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -3939,61 +4006,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F27FAEFF-543C-4C30-A571-905BD321BEF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E9A4B38-4D52-46C0-9803-4EB30CC27F1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2021-03-04T14:13:47+00:00</Document_x0020_Creation_x0020_Date>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3227138-1B8A-4733-BA76-D224862EAA4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{658CB8BC-C675-45A5-9E4E-E3C3C47B95A1}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D04565B-B583-4D5E-81D8-147E78B4962D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4013,33 +4056,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3227138-1B8A-4733-BA76-D224862EAA4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E9A4B38-4D52-46C0-9803-4EB30CC27F1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F27FAEFF-543C-4C30-A571-905BD321BEF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>